<commit_message>
commiting after fixing SessionNotFoundException: Session ID is null.Using WebDriver after calling quit()? (Selenium)
</commit_message>
<xml_diff>
--- a/src/test/resources/com/hrm/data/ProjectData.xlsx
+++ b/src/test/resources/com/hrm/data/ProjectData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3B6627B9-6040-4A9E-9B34-682C1408987F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CBBD3C71-49C2-4AF5-8D0B-5B5E7C038281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{635658EA-B9CD-4037-A46B-26225CC9A0A7}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Data Driven Testing Implemented
</commit_message>
<xml_diff>
--- a/src/test/resources/com/hrm/data/ProjectData.xlsx
+++ b/src/test/resources/com/hrm/data/ProjectData.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CBBD3C71-49C2-4AF5-8D0B-5B5E7C038281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{994D7753-063E-490C-AD39-16D749502F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{635658EA-B9CD-4037-A46B-26225CC9A0A7}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{635658EA-B9CD-4037-A46B-26225CC9A0A7}"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
-    <sheet name="RELEASE" sheetId="2" r:id="rId2"/>
-    <sheet name="PRODUCTION" sheetId="3" r:id="rId3"/>
-    <sheet name="DEV" sheetId="4" r:id="rId4"/>
+    <sheet name="LoginTestData" sheetId="5" r:id="rId2"/>
+    <sheet name="RELEASE" sheetId="2" r:id="rId3"/>
+    <sheet name="PRODUCTION" sheetId="3" r:id="rId4"/>
+    <sheet name="DEV" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L33"/>
+  <oleSize ref="A1:Q33"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
   <si>
     <t>URL</t>
   </si>
@@ -60,13 +61,43 @@
   </si>
   <si>
     <t>PROD</t>
+  </si>
+  <si>
+    <t>TC_ID</t>
+  </si>
+  <si>
+    <t>Scenario_ID</t>
+  </si>
+  <si>
+    <t>TC00001</t>
+  </si>
+  <si>
+    <t>S_ID_00001</t>
+  </si>
+  <si>
+    <t>TC00002</t>
+  </si>
+  <si>
+    <t>TC00003</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>WrongUsername</t>
+  </si>
+  <si>
+    <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>wrongPassword</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +120,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFEB0910"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -107,10 +158,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -118,8 +170,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -434,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708C47A5-9A0F-430B-A619-246DADB1DF73}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +523,7 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
@@ -482,12 +537,107 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{AEF8235F-D16D-4BFA-B2FB-A8633DB5BAFC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEF9D94-4004-4522-B79D-1A9A2C5DC93E}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE818315-B54A-408B-B461-1D1CEC8A140C}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -536,7 +686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5EB4650-3B26-436D-9C28-A956F88839F8}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -585,7 +735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578C4060-EFD7-404D-9FD4-10BD6EEA8D27}">
   <dimension ref="A1:E2"/>
   <sheetViews>

</xml_diff>